<commit_message>
fix: remove cohorts from tablename and remove duplicate recruit_age
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/2_0/2_0_non_rep.xlsx
+++ b/R/data/dictionaries/core/2_0/2_0_non_rep.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Library/Containers/com.microsoft.Excel/Data/Downloads/trimester/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340AB81F-B15A-CF4A-89F4-098DD9B01940}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF00FB7-85A6-8446-B774-194C9F2B9BAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="828">
   <si>
     <t>name</t>
   </si>
@@ -2923,10 +2923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D318"/>
+  <dimension ref="A1:D317"/>
   <sheetViews>
-    <sheetView topLeftCell="A289" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C317" sqref="C317"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105:XFD105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4392,77 +4392,77 @@
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1">
       <c r="A105" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1">
       <c r="A106" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1">
       <c r="A107" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1">
       <c r="A108" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1">
       <c r="A109" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>315</v>
@@ -4471,40 +4471,40 @@
         <v>324</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1">
       <c r="A111" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1">
       <c r="A112" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1">
       <c r="A113" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>315</v>
@@ -4513,40 +4513,40 @@
         <v>325</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="A114" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1">
       <c r="A115" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>314</v>
@@ -4555,12 +4555,12 @@
         <v>317</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>314</v>
@@ -4569,12 +4569,12 @@
         <v>317</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1">
       <c r="A118" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>314</v>
@@ -4583,26 +4583,26 @@
         <v>317</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>317</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1">
       <c r="A120" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>315</v>
@@ -4611,40 +4611,40 @@
         <v>317</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="A121" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>317</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1">
       <c r="A122" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1">
       <c r="A123" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>315</v>
@@ -4653,12 +4653,12 @@
         <v>327</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1">
       <c r="A124" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>315</v>
@@ -4667,12 +4667,12 @@
         <v>327</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1">
       <c r="A125" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>315</v>
@@ -4681,12 +4681,12 @@
         <v>327</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1">
       <c r="A126" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>315</v>
@@ -4695,40 +4695,40 @@
         <v>327</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1">
       <c r="A127" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1">
       <c r="A128" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1">
       <c r="A129" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>315</v>
@@ -4737,12 +4737,12 @@
         <v>329</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1">
       <c r="A130" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>315</v>
@@ -4751,12 +4751,12 @@
         <v>329</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1">
       <c r="A131" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>315</v>
@@ -4765,12 +4765,12 @@
         <v>329</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="A132" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>315</v>
@@ -4779,12 +4779,12 @@
         <v>329</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1">
       <c r="A133" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>315</v>
@@ -4793,12 +4793,12 @@
         <v>329</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1">
       <c r="A134" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>315</v>
@@ -4807,12 +4807,12 @@
         <v>329</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>315</v>
@@ -4821,12 +4821,12 @@
         <v>329</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1">
       <c r="A136" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>315</v>
@@ -4835,12 +4835,12 @@
         <v>329</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>315</v>
@@ -4849,12 +4849,12 @@
         <v>329</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>315</v>
@@ -4863,12 +4863,12 @@
         <v>329</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>315</v>
@@ -4877,12 +4877,12 @@
         <v>329</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1">
       <c r="A140" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>315</v>
@@ -4891,12 +4891,12 @@
         <v>329</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1">
       <c r="A141" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>315</v>
@@ -4905,12 +4905,12 @@
         <v>329</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15" customHeight="1">
       <c r="A142" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>315</v>
@@ -4919,12 +4919,12 @@
         <v>329</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1">
       <c r="A143" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>315</v>
@@ -4933,40 +4933,40 @@
         <v>329</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1">
       <c r="A144" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1">
       <c r="A145" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" customHeight="1">
       <c r="A146" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>315</v>
@@ -4975,26 +4975,26 @@
         <v>331</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1">
       <c r="A147" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1">
       <c r="A148" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>315</v>
@@ -5003,26 +5003,26 @@
         <v>332</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1">
       <c r="A149" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1">
       <c r="A150" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>315</v>
@@ -5031,12 +5031,12 @@
         <v>333</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1">
       <c r="A151" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>315</v>
@@ -5045,26 +5045,26 @@
         <v>333</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1">
       <c r="A152" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1">
       <c r="A153" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>315</v>
@@ -5078,7 +5078,7 @@
     </row>
     <row r="154" spans="1:4" ht="15" customHeight="1">
       <c r="A154" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>315</v>
@@ -5087,12 +5087,12 @@
         <v>332</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" customHeight="1">
       <c r="A155" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>315</v>
@@ -5101,26 +5101,26 @@
         <v>332</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" customHeight="1">
       <c r="A156" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15" customHeight="1">
       <c r="A157" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>315</v>
@@ -5129,40 +5129,40 @@
         <v>325</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15" customHeight="1">
       <c r="A158" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15" customHeight="1">
       <c r="A159" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" customHeight="1">
       <c r="A160" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>315</v>
@@ -5171,12 +5171,12 @@
         <v>334</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15" customHeight="1">
       <c r="A161" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>315</v>
@@ -5185,12 +5185,12 @@
         <v>334</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15" customHeight="1">
       <c r="A162" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>315</v>
@@ -5199,12 +5199,12 @@
         <v>334</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15" customHeight="1">
       <c r="A163" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>315</v>
@@ -5213,12 +5213,12 @@
         <v>334</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15" customHeight="1">
       <c r="A164" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>315</v>
@@ -5227,12 +5227,12 @@
         <v>334</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15" customHeight="1">
       <c r="A165" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>315</v>
@@ -5241,12 +5241,12 @@
         <v>334</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>315</v>
@@ -5255,12 +5255,12 @@
         <v>334</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>315</v>
@@ -5269,12 +5269,12 @@
         <v>334</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15" customHeight="1">
       <c r="A168" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>315</v>
@@ -5283,12 +5283,12 @@
         <v>334</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15" customHeight="1">
       <c r="A169" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>315</v>
@@ -5297,12 +5297,12 @@
         <v>334</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15" customHeight="1">
       <c r="A170" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>315</v>
@@ -5311,26 +5311,26 @@
         <v>334</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15" customHeight="1">
       <c r="A172" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>315</v>
@@ -5339,26 +5339,26 @@
         <v>335</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15" customHeight="1">
       <c r="A173" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15" customHeight="1">
       <c r="A174" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>315</v>
@@ -5367,26 +5367,26 @@
         <v>336</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15" customHeight="1">
       <c r="A175" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15" customHeight="1">
       <c r="A176" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>314</v>
@@ -5395,26 +5395,26 @@
         <v>317</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15" customHeight="1">
       <c r="A177" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1">
       <c r="A178" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>315</v>
@@ -5423,12 +5423,12 @@
         <v>337</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15" customHeight="1">
       <c r="A179" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>315</v>
@@ -5437,26 +5437,26 @@
         <v>337</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15" customHeight="1">
       <c r="A180" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15" customHeight="1">
       <c r="A181" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>315</v>
@@ -5465,26 +5465,26 @@
         <v>338</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15" customHeight="1">
       <c r="A182" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15" customHeight="1">
       <c r="A183" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>314</v>
@@ -5493,40 +5493,40 @@
         <v>317</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15" customHeight="1">
       <c r="A184" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>317</v>
+        <v>335</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15" customHeight="1">
       <c r="A185" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15" customHeight="1">
       <c r="A186" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>314</v>
@@ -5535,40 +5535,40 @@
         <v>317</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15" customHeight="1">
       <c r="A187" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>317</v>
+        <v>339</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15" customHeight="1">
       <c r="A188" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15" customHeight="1">
       <c r="A189" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>315</v>
@@ -5577,40 +5577,40 @@
         <v>340</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15" customHeight="1">
       <c r="A190" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15" customHeight="1">
       <c r="A191" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15" customHeight="1">
       <c r="A192" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>315</v>
@@ -5619,26 +5619,26 @@
         <v>332</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1">
       <c r="A193" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15" customHeight="1">
       <c r="A194" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>315</v>
@@ -5647,12 +5647,12 @@
         <v>342</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15" customHeight="1">
       <c r="A195" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>315</v>
@@ -5661,26 +5661,26 @@
         <v>342</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15" customHeight="1">
       <c r="A196" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15" customHeight="1">
       <c r="A197" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>315</v>
@@ -5689,12 +5689,12 @@
         <v>334</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15" customHeight="1">
       <c r="A198" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>315</v>
@@ -5703,26 +5703,26 @@
         <v>334</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15" customHeight="1">
       <c r="A199" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="15" customHeight="1">
       <c r="A200" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>315</v>
@@ -5731,12 +5731,12 @@
         <v>343</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15" customHeight="1">
       <c r="A201" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>315</v>
@@ -5745,40 +5745,40 @@
         <v>343</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15" customHeight="1">
       <c r="A202" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15" customHeight="1">
       <c r="A203" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15" customHeight="1">
       <c r="A204" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>315</v>
@@ -5787,12 +5787,12 @@
         <v>344</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15" customHeight="1">
       <c r="A205" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>315</v>
@@ -5801,12 +5801,12 @@
         <v>344</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15" customHeight="1">
       <c r="A206" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>315</v>
@@ -5815,12 +5815,12 @@
         <v>344</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15" customHeight="1">
       <c r="A207" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>315</v>
@@ -5829,12 +5829,12 @@
         <v>344</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15" customHeight="1">
       <c r="A208" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>315</v>
@@ -5843,12 +5843,12 @@
         <v>344</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1">
       <c r="A209" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>315</v>
@@ -5857,12 +5857,12 @@
         <v>344</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15" customHeight="1">
       <c r="A210" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>315</v>
@@ -5871,12 +5871,12 @@
         <v>344</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15" customHeight="1">
       <c r="A211" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>315</v>
@@ -5885,12 +5885,12 @@
         <v>344</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="15" customHeight="1">
       <c r="A212" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>315</v>
@@ -5899,12 +5899,12 @@
         <v>344</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="15" customHeight="1">
       <c r="A213" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>315</v>
@@ -5913,12 +5913,12 @@
         <v>344</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="15" customHeight="1">
       <c r="A214" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>315</v>
@@ -5927,12 +5927,12 @@
         <v>344</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="15" customHeight="1">
       <c r="A215" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>315</v>
@@ -5941,12 +5941,12 @@
         <v>344</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="15" customHeight="1">
       <c r="A216" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>315</v>
@@ -5955,12 +5955,12 @@
         <v>344</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15" customHeight="1">
       <c r="A217" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>315</v>
@@ -5969,12 +5969,12 @@
         <v>344</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="15" customHeight="1">
       <c r="A218" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>315</v>
@@ -5983,12 +5983,12 @@
         <v>344</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15" customHeight="1">
       <c r="A219" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>315</v>
@@ -5997,12 +5997,12 @@
         <v>344</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15" customHeight="1">
       <c r="A220" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>315</v>
@@ -6011,54 +6011,54 @@
         <v>344</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15" customHeight="1">
       <c r="A221" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15" customHeight="1">
       <c r="A222" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>317</v>
+        <v>345</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15" customHeight="1">
       <c r="A223" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15" customHeight="1">
       <c r="A224" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>315</v>
@@ -6067,12 +6067,12 @@
         <v>344</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15" customHeight="1">
       <c r="A225" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>315</v>
@@ -6081,12 +6081,12 @@
         <v>344</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15" customHeight="1">
       <c r="A226" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>315</v>
@@ -6095,12 +6095,12 @@
         <v>344</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15" customHeight="1">
       <c r="A227" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>315</v>
@@ -6109,12 +6109,12 @@
         <v>344</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15" customHeight="1">
       <c r="A228" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>315</v>
@@ -6123,12 +6123,12 @@
         <v>344</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15" customHeight="1">
       <c r="A229" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>315</v>
@@ -6137,12 +6137,12 @@
         <v>344</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="15" customHeight="1">
       <c r="A230" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>315</v>
@@ -6151,12 +6151,12 @@
         <v>344</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="15" customHeight="1">
       <c r="A231" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>315</v>
@@ -6165,12 +6165,12 @@
         <v>344</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15" customHeight="1">
       <c r="A232" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>315</v>
@@ -6179,12 +6179,12 @@
         <v>344</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1">
       <c r="A233" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>315</v>
@@ -6193,12 +6193,12 @@
         <v>344</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="15" customHeight="1">
       <c r="A234" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>315</v>
@@ -6207,12 +6207,12 @@
         <v>344</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15" customHeight="1">
       <c r="A235" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>315</v>
@@ -6221,12 +6221,12 @@
         <v>344</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15" customHeight="1">
       <c r="A236" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>315</v>
@@ -6235,12 +6235,12 @@
         <v>344</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15" customHeight="1">
       <c r="A237" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>315</v>
@@ -6249,12 +6249,12 @@
         <v>344</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15" customHeight="1">
       <c r="A238" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>315</v>
@@ -6263,12 +6263,12 @@
         <v>344</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15" customHeight="1">
       <c r="A239" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>315</v>
@@ -6277,12 +6277,12 @@
         <v>344</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15" customHeight="1">
       <c r="A240" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>315</v>
@@ -6291,54 +6291,54 @@
         <v>344</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="15" customHeight="1">
       <c r="A241" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="15" customHeight="1">
       <c r="A242" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="15" customHeight="1">
       <c r="A243" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B243" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15" customHeight="1">
       <c r="A244" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>315</v>
@@ -6347,12 +6347,12 @@
         <v>344</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="15" customHeight="1">
       <c r="A245" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>315</v>
@@ -6361,12 +6361,12 @@
         <v>344</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1">
       <c r="A246" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>315</v>
@@ -6375,12 +6375,12 @@
         <v>344</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="15" customHeight="1">
       <c r="A247" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>315</v>
@@ -6389,12 +6389,12 @@
         <v>344</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15" customHeight="1">
       <c r="A248" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>315</v>
@@ -6403,12 +6403,12 @@
         <v>344</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15" customHeight="1">
       <c r="A249" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>315</v>
@@ -6417,12 +6417,12 @@
         <v>344</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15" customHeight="1">
       <c r="A250" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>315</v>
@@ -6431,12 +6431,12 @@
         <v>344</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15" customHeight="1">
       <c r="A251" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>315</v>
@@ -6445,12 +6445,12 @@
         <v>344</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15" customHeight="1">
       <c r="A252" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>315</v>
@@ -6459,12 +6459,12 @@
         <v>344</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15" customHeight="1">
       <c r="A253" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>315</v>
@@ -6473,12 +6473,12 @@
         <v>344</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15" customHeight="1">
       <c r="A254" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>315</v>
@@ -6487,12 +6487,12 @@
         <v>344</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15" customHeight="1">
       <c r="A255" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>315</v>
@@ -6501,12 +6501,12 @@
         <v>344</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15" customHeight="1">
       <c r="A256" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>315</v>
@@ -6515,12 +6515,12 @@
         <v>344</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15" customHeight="1">
       <c r="A257" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>315</v>
@@ -6529,12 +6529,12 @@
         <v>344</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15" customHeight="1">
       <c r="A258" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>315</v>
@@ -6543,12 +6543,12 @@
         <v>344</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15" customHeight="1">
       <c r="A259" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>315</v>
@@ -6557,12 +6557,12 @@
         <v>344</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15" customHeight="1">
       <c r="A260" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>315</v>
@@ -6571,96 +6571,96 @@
         <v>344</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15" customHeight="1">
       <c r="A261" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15" customHeight="1">
       <c r="A262" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15" customHeight="1">
       <c r="A263" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15" customHeight="1">
       <c r="A264" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15" customHeight="1">
       <c r="A265" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15" customHeight="1">
       <c r="A266" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15" customHeight="1">
       <c r="A267" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>315</v>
@@ -6669,12 +6669,12 @@
         <v>349</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15" customHeight="1">
       <c r="A268" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>315</v>
@@ -6683,116 +6683,116 @@
         <v>349</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15" customHeight="1">
       <c r="A269" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15" customHeight="1">
       <c r="A270" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15" customHeight="1">
       <c r="A271" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="15" customHeight="1">
       <c r="A272" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="15" customHeight="1">
       <c r="A273" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="15" customHeight="1">
       <c r="A274" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="15" customHeight="1">
       <c r="A275" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15" customHeight="1">
       <c r="A276" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>627</v>
@@ -6800,21 +6800,21 @@
     </row>
     <row r="277" spans="1:4" ht="15" customHeight="1">
       <c r="A277" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15" customHeight="1">
       <c r="A278" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>315</v>
@@ -6823,12 +6823,12 @@
         <v>349</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="15" customHeight="1">
       <c r="A279" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B279" s="2" t="s">
         <v>315</v>
@@ -6837,32 +6837,32 @@
         <v>349</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="15" customHeight="1">
       <c r="A280" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15" customHeight="1">
       <c r="A281" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>631</v>
@@ -6870,27 +6870,27 @@
     </row>
     <row r="282" spans="1:4" ht="15" customHeight="1">
       <c r="A282" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="15" customHeight="1">
       <c r="A283" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>632</v>
@@ -6898,55 +6898,55 @@
     </row>
     <row r="284" spans="1:4" ht="15" customHeight="1">
       <c r="A284" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15" customHeight="1">
       <c r="A285" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="15" customHeight="1">
       <c r="A286" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15" customHeight="1">
       <c r="A287" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>635</v>
@@ -6954,21 +6954,21 @@
     </row>
     <row r="288" spans="1:4" ht="15" customHeight="1">
       <c r="A288" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>635</v>
+        <v>618</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="15" customHeight="1">
       <c r="A289" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>315</v>
@@ -6977,12 +6977,12 @@
         <v>349</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>618</v>
+        <v>636</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15" customHeight="1">
       <c r="A290" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>315</v>
@@ -6991,32 +6991,32 @@
         <v>349</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15" customHeight="1">
       <c r="A291" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15" customHeight="1">
       <c r="A292" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>638</v>
@@ -7024,27 +7024,27 @@
     </row>
     <row r="293" spans="1:4" ht="15" customHeight="1">
       <c r="A293" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15" customHeight="1">
       <c r="A294" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>639</v>
@@ -7052,35 +7052,35 @@
     </row>
     <row r="295" spans="1:4" ht="15" customHeight="1">
       <c r="A295" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15" customHeight="1">
       <c r="A296" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>350</v>
+        <v>317</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15" customHeight="1">
       <c r="A297" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>314</v>
@@ -7089,26 +7089,26 @@
         <v>317</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15" customHeight="1">
       <c r="A298" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>317</v>
+        <v>351</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15" customHeight="1">
       <c r="A299" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>315</v>
@@ -7117,12 +7117,12 @@
         <v>351</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15" customHeight="1">
       <c r="A300" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>315</v>
@@ -7131,26 +7131,26 @@
         <v>351</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15" customHeight="1">
       <c r="A301" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="15" customHeight="1">
       <c r="A302" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>315</v>
@@ -7159,26 +7159,26 @@
         <v>352</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="15" customHeight="1">
       <c r="A303" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="15" customHeight="1">
       <c r="A304" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>315</v>
@@ -7187,12 +7187,12 @@
         <v>351</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15" customHeight="1">
       <c r="A305" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>315</v>
@@ -7201,12 +7201,12 @@
         <v>351</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="15" customHeight="1">
       <c r="A306" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>315</v>
@@ -7215,26 +7215,26 @@
         <v>351</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15" customHeight="1">
       <c r="A307" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="15" customHeight="1">
       <c r="A308" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>315</v>
@@ -7243,40 +7243,40 @@
         <v>352</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="15" customHeight="1">
       <c r="A309" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="15" customHeight="1">
       <c r="A310" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="15" customHeight="1">
       <c r="A311" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>314</v>
@@ -7285,12 +7285,12 @@
         <v>317</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="15" customHeight="1">
       <c r="A312" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>314</v>
@@ -7299,90 +7299,76 @@
         <v>317</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="15" customHeight="1">
-      <c r="A313" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B313" s="2" t="s">
+      <c r="A313" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B313" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C313" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="D313" s="2" t="s">
-        <v>651</v>
+      <c r="C313" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D313" s="3" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="15" customHeight="1">
       <c r="A314" s="4" t="s">
-        <v>104</v>
+        <v>825</v>
       </c>
       <c r="B314" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C314" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="D314" s="3" t="s">
-        <v>457</v>
+      <c r="C314" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D314" s="5" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="15" customHeight="1">
       <c r="A315" s="4" t="s">
-        <v>825</v>
-      </c>
-      <c r="B315" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="B315" s="4" t="s">
         <v>314</v>
       </c>
       <c r="C315" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="D315" s="5" t="s">
-        <v>819</v>
+        <v>823</v>
+      </c>
+      <c r="D315" s="3" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="15" customHeight="1">
       <c r="A316" s="4" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="B316" s="4" t="s">
         <v>314</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>823</v>
+        <v>317</v>
       </c>
       <c r="D316" s="3" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="15" customHeight="1">
       <c r="A317" s="4" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B317" s="4" t="s">
         <v>314</v>
       </c>
       <c r="C317" s="5" t="s">
-        <v>317</v>
+        <v>822</v>
       </c>
       <c r="D317" s="3" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="318" spans="1:4" ht="15" customHeight="1">
-      <c r="A318" s="4" t="s">
-        <v>827</v>
-      </c>
-      <c r="B318" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="C318" s="5" t="s">
-        <v>822</v>
-      </c>
-      <c r="D318" s="3" t="s">
         <v>821</v>
       </c>
     </row>
@@ -7398,7 +7384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C309" sqref="C309"/>
     </sheetView>

</xml_diff>